<commit_message>
Criação das abas de Main e Shrine Quests
</commit_message>
<xml_diff>
--- a/zelda-botw-checklist/data/Template.xlsx
+++ b/zelda-botw-checklist/data/Template.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlon\Projetos\zelda-botw-tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlon\Projetos\zelda-botw-checklist\zelda-botw-checklist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A59E25-2203-45F6-9FAE-9C897E32232A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4768A3F3-92EF-45B1-AB55-92730F67EBB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{430C5E47-7444-4596-8215-16F7A9424B2C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Side Quests" sheetId="1" r:id="rId1"/>
-    <sheet name="Savegame_Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Main Quests" sheetId="3" r:id="rId1"/>
+    <sheet name="Side Quests" sheetId="1" r:id="rId2"/>
+    <sheet name="Shrine Quests" sheetId="4" r:id="rId3"/>
+    <sheet name="Savegame_Data" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="230">
   <si>
     <t>Wild Horses</t>
   </si>
@@ -416,6 +418,312 @@
   </si>
   <si>
     <t>Zelda BOTW Checklist - Side Quests</t>
+  </si>
+  <si>
+    <t>A Gift for the Great Fairy</t>
+  </si>
+  <si>
+    <t>Tabantha Bridge Stable</t>
+  </si>
+  <si>
+    <t>Zelda BOTW Checklist - Main Quests</t>
+  </si>
+  <si>
+    <t>Follow the Sheikah Slate</t>
+  </si>
+  <si>
+    <t>The Isolated Plateau</t>
+  </si>
+  <si>
+    <t>Seek Out Impa</t>
+  </si>
+  <si>
+    <t>Locked Mementos</t>
+  </si>
+  <si>
+    <t>Find the Fairy Fountain</t>
+  </si>
+  <si>
+    <t>Captured Memories</t>
+  </si>
+  <si>
+    <t>Free the Divine Beasts</t>
+  </si>
+  <si>
+    <t>Reach Zora's Domain</t>
+  </si>
+  <si>
+    <t>Divine Beast Vah Ruta</t>
+  </si>
+  <si>
+    <t>Divine Beast Vah Rudania</t>
+  </si>
+  <si>
+    <t>Forbidden City Entry</t>
+  </si>
+  <si>
+    <t>Divine Beast Vah Naboris</t>
+  </si>
+  <si>
+    <t>Divine Beast Vah Medoh</t>
+  </si>
+  <si>
+    <t>The Hero's Sword</t>
+  </si>
+  <si>
+    <t>Destroy Ganon</t>
+  </si>
+  <si>
+    <t>EX The Champions' Ballad</t>
+  </si>
+  <si>
+    <t>EX Champion Urbosa's Song</t>
+  </si>
+  <si>
+    <t>EX Champion Daruk's Song</t>
+  </si>
+  <si>
+    <t>EX Champion Revali's Song</t>
+  </si>
+  <si>
+    <t>EX Champion Mipha's Song</t>
+  </si>
+  <si>
+    <t>Great Plateau</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Lanayru Tower</t>
+  </si>
+  <si>
+    <t>Hyrule Castle</t>
+  </si>
+  <si>
+    <t>The Great Plateau</t>
+  </si>
+  <si>
+    <t>Wasteland Region</t>
+  </si>
+  <si>
+    <t>Eldin Region</t>
+  </si>
+  <si>
+    <t>Hebra Region</t>
+  </si>
+  <si>
+    <t>Lanayru Region</t>
+  </si>
+  <si>
+    <t>The Stolen Heirloom</t>
+  </si>
+  <si>
+    <t>Watch Out for the Flowers</t>
+  </si>
+  <si>
+    <t>Hylia River</t>
+  </si>
+  <si>
+    <t>Secret of the Cedars</t>
+  </si>
+  <si>
+    <t>The Crowned Beast</t>
+  </si>
+  <si>
+    <t>The Cursed Statue</t>
+  </si>
+  <si>
+    <t>The Spring of Wisdom</t>
+  </si>
+  <si>
+    <t>Rabia Plain</t>
+  </si>
+  <si>
+    <t>Fort Hateno</t>
+  </si>
+  <si>
+    <t>Master of the Wind</t>
+  </si>
+  <si>
+    <t>The Ceremonial Song</t>
+  </si>
+  <si>
+    <t>Horon Lagoon</t>
+  </si>
+  <si>
+    <t>A Brother's Roast</t>
+  </si>
+  <si>
+    <t>A Landscape of a Stable</t>
+  </si>
+  <si>
+    <t>The Gut Check Challenge</t>
+  </si>
+  <si>
+    <t>Cliffside Etchings</t>
+  </si>
+  <si>
+    <t>Sign of the Shadow</t>
+  </si>
+  <si>
+    <t>Test of Will</t>
+  </si>
+  <si>
+    <t>Secret of the Snowy Peaks</t>
+  </si>
+  <si>
+    <t>The Eye of the Sandstorm</t>
+  </si>
+  <si>
+    <t>The Desert Labyrinth</t>
+  </si>
+  <si>
+    <t>The Perfect Drink</t>
+  </si>
+  <si>
+    <t>The Seven Heroines</t>
+  </si>
+  <si>
+    <t>The Silent Swordswomen</t>
+  </si>
+  <si>
+    <t>The Undefeated Champ</t>
+  </si>
+  <si>
+    <t>Gerudo Tower</t>
+  </si>
+  <si>
+    <t>Mount Nabooru</t>
+  </si>
+  <si>
+    <t>Mountain Peak Log Cabin</t>
+  </si>
+  <si>
+    <t>South Lomei Labyrinth</t>
+  </si>
+  <si>
+    <t>East Barrens</t>
+  </si>
+  <si>
+    <t>Sand-Seal Rally</t>
+  </si>
+  <si>
+    <t>Recital at Warbler's Nest</t>
+  </si>
+  <si>
+    <t>The Ancient Rito Song</t>
+  </si>
+  <si>
+    <t>Warbler's Nest</t>
+  </si>
+  <si>
+    <t>Mayro</t>
+  </si>
+  <si>
+    <t>Bayge</t>
+  </si>
+  <si>
+    <t>Guardian Slideshow</t>
+  </si>
+  <si>
+    <t>The Serpent's Jaws</t>
+  </si>
+  <si>
+    <t>Puffer Beach</t>
+  </si>
+  <si>
+    <t>Pagos Woods</t>
+  </si>
+  <si>
+    <t>A Fragmented Monument</t>
+  </si>
+  <si>
+    <t>A Song of Storms</t>
+  </si>
+  <si>
+    <t>Stranded on Eventide</t>
+  </si>
+  <si>
+    <t>The Three Giant Brothers</t>
+  </si>
+  <si>
+    <t>Palmorae Ruins</t>
+  </si>
+  <si>
+    <t>Calora Lake</t>
+  </si>
+  <si>
+    <t>Eventide Island</t>
+  </si>
+  <si>
+    <t>Mount Taran</t>
+  </si>
+  <si>
+    <t>Into the Vortex</t>
+  </si>
+  <si>
+    <t>The Skull's Eye</t>
+  </si>
+  <si>
+    <t>The Spring of Power</t>
+  </si>
+  <si>
+    <t>Malin Bay</t>
+  </si>
+  <si>
+    <t>Akkala Ancient Tech Lab</t>
+  </si>
+  <si>
+    <t>The Bird in the Mountains</t>
+  </si>
+  <si>
+    <t>Trial on the Cliff</t>
+  </si>
+  <si>
+    <t>North Lomei Labyrinth</t>
+  </si>
+  <si>
+    <t>Shrouded Shrine</t>
+  </si>
+  <si>
+    <t>The Lost Pilgrimage</t>
+  </si>
+  <si>
+    <t>The Test of Wood</t>
+  </si>
+  <si>
+    <t>Trial of Second Sight</t>
+  </si>
+  <si>
+    <t>Thyplo Ruins</t>
+  </si>
+  <si>
+    <t>The Two Rings</t>
+  </si>
+  <si>
+    <t>Trial of Thunder</t>
+  </si>
+  <si>
+    <t>Under a Red Moon</t>
+  </si>
+  <si>
+    <t>West Hyrule Plains</t>
+  </si>
+  <si>
+    <t>Thundra Plateau</t>
+  </si>
+  <si>
+    <t>Hyrule Ridge</t>
+  </si>
+  <si>
+    <t>Trial of the Labyrinth</t>
+  </si>
+  <si>
+    <t>Lomei Labyrinth Island</t>
+  </si>
+  <si>
+    <t>Zelda BOTW Checklist - Shrine Quests</t>
   </si>
 </sst>
 </file>
@@ -527,7 +835,231 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF4C7B38"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF981F1F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF4C7B38"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF981F1F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF4C7B38"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF981F1F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF4C7B38"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF981F1F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF4C7B38"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF981F1F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF4C7B38"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF981F1F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF4C7B38"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF981F1F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF4C7B38"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF981F1F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -874,12 +1406,319 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5121A2F7-F462-4159-B690-1D2F6D8773DE}">
+  <dimension ref="B1:L19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4" t="str">
+        <f>"| Total Quests: 20 | Completed : "&amp;COUNTIF(B5:F19,"Yes")&amp;" | Remaining: "&amp;20-COUNTIF(B5:F19,"Yes")&amp;" |"</f>
+        <v>| Total Quests: 20 | Completed : 0 | Remaining: 20 |</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="str">
+        <f>"Main Quests ("&amp;COUNTIF(B5:B19,"Yes")&amp;"/15)"</f>
+        <v>Main Quests (0/15)</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="F4" s="6" t="str">
+        <f>"Main Quests (DLC) ("&amp;COUNTIF(F5:F14,"Yes")&amp;"/5)"</f>
+        <v>Main Quests (DLC) (0/5)</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="e">
+        <f>IF(VLOOKUP(C5,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="2" t="e">
+        <f>IF(VLOOKUP(G5,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="e">
+        <f>IF(VLOOKUP(C6,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="2" t="e">
+        <f>IF(VLOOKUP(G6,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="e">
+        <f>IF(VLOOKUP(C7,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="2" t="e">
+        <f>IF(VLOOKUP(G7,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="e">
+        <f>IF(VLOOKUP(C8,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="e">
+        <f>IF(VLOOKUP(G8,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="e">
+        <f>IF(VLOOKUP(C9,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="e">
+        <f>IF(VLOOKUP(G9,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="e">
+        <f>IF(VLOOKUP(C10,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="e">
+        <f>IF(VLOOKUP(C11,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="e">
+        <f>IF(VLOOKUP(C12,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="e">
+        <f>IF(VLOOKUP(C13,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="e">
+        <f>IF(VLOOKUP(C14,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="e">
+        <f>IF(VLOOKUP(C15,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="e">
+        <f>IF(VLOOKUP(C16,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="e">
+        <f>IF(VLOOKUP(C17,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="e">
+        <f>IF(VLOOKUP(C18,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="e">
+        <f>IF(VLOOKUP(C19,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B2:G2 I2:L2 B3:L1048576">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96528F81-0B6F-46FD-B653-1A103D51BB66}">
   <dimension ref="B1:L48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,8 +1981,8 @@
         <v>24</v>
       </c>
       <c r="J11" s="6" t="str">
-        <f>"Central Region ("&amp;COUNTIF(J12:J15,"Yes")&amp;"/4)"</f>
-        <v>Central Region (0/4)</v>
+        <f>"Eldin Region ("&amp;COUNTIF(J12:J15,"Yes")&amp;"/4)"</f>
+        <v>Eldin Region (0/4)</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -1292,8 +2131,8 @@
         <v>65</v>
       </c>
       <c r="J17" s="6" t="str">
-        <f>"Tabantha Region ("&amp;COUNTIF(J18:J22,"Yes")&amp;"/5)"</f>
-        <v>Tabantha Region (0/5)</v>
+        <f>"Tabantha Region ("&amp;COUNTIF(J18:J22,"Yes")&amp;"/6)"</f>
+        <v>Tabantha Region (0/6)</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
@@ -1479,6 +2318,16 @@
       <c r="H23" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="J23" s="2" t="e">
+        <f>IF(VLOOKUP(K23,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="e">
@@ -1501,12 +2350,6 @@
       <c r="H24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J24" s="6" t="str">
-        <f>"Lake Region ("&amp;COUNTIF(J25:J26,"Yes")&amp;"/2)"</f>
-        <v>Lake Region (0/2)</v>
-      </c>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="e">
@@ -1529,16 +2372,12 @@
       <c r="H25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J25" s="2" t="e">
-        <f>IF(VLOOKUP(K25,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="J25" s="6" t="str">
+        <f>"Lake Region ("&amp;COUNTIF(J26:J27,"Yes")&amp;"/2)"</f>
+        <v>Lake Region (0/2)</v>
+      </c>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="e">
@@ -1566,10 +2405,10 @@
         <v>#N/A</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
@@ -1582,6 +2421,16 @@
       </c>
       <c r="H27" s="1" t="s">
         <v>68</v>
+      </c>
+      <c r="J27" s="2" t="e">
+        <f>IF(VLOOKUP(K27,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
@@ -1603,12 +2452,6 @@
       <c r="H28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J28" s="6" t="str">
-        <f>"Lake Region ("&amp;COUNTIF(J29:J32,"Yes")&amp;"/4)"</f>
-        <v>Lake Region (0/4)</v>
-      </c>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="e">
@@ -1621,16 +2464,12 @@
       <c r="D29" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J29" s="2" t="e">
-        <f>IF(VLOOKUP(K29,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="J29" s="6" t="str">
+        <f>"Akkala Region ("&amp;COUNTIF(J30:J33,"Yes")&amp;"/4)"</f>
+        <v>Akkala Region (0/4)</v>
+      </c>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="e">
@@ -1654,10 +2493,10 @@
         <v>#N/A</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
@@ -1686,10 +2525,10 @@
         <v>#N/A</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
@@ -1718,7 +2557,7 @@
         <v>#N/A</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>106</v>
@@ -1745,6 +2584,16 @@
       <c r="H33" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="J33" s="2" t="e">
+        <f>IF(VLOOKUP(K33,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F34" s="2" t="e">
@@ -1757,12 +2606,6 @@
       <c r="H34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J34" s="6" t="str">
-        <f>"Hebra Region ("&amp;COUNTIF(J35:J36,"Yes")&amp;"/2)"</f>
-        <v>Hebra Region (0/2)</v>
-      </c>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="str">
@@ -1781,16 +2624,12 @@
       <c r="H35" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J35" s="2" t="e">
-        <f>IF(VLOOKUP(K35,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="J35" s="6" t="str">
+        <f>"Hebra Region ("&amp;COUNTIF(J36:J37,"Yes")&amp;"/2)"</f>
+        <v>Hebra Region (0/2)</v>
+      </c>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="e">
@@ -1818,10 +2657,10 @@
         <v>#N/A</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
@@ -1844,6 +2683,16 @@
       </c>
       <c r="H37" s="1" t="s">
         <v>99</v>
+      </c>
+      <c r="J37" s="2" t="e">
+        <f>IF(VLOOKUP(K37,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
@@ -1988,17 +2837,17 @@
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J25:L25"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="F30:H30"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="J35:L35"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:L1048576 B2:G2 I2:L2">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2:G2 I2:L2 B38:L1048576 B24:I37 J25:L37 B3:L23">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2007,7 +2856,668 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1057E3-A70F-481D-8E8E-C615561C98F9}">
+  <dimension ref="B1:L26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O34" sqref="O34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4" t="str">
+        <f>"| Total Quests: 42 | Completed : "&amp;COUNTIF(B5:J37,"Yes")&amp;" | Remaining: "&amp;42-COUNTIF(B5:J37,"Yes")&amp;" |"</f>
+        <v>| Total Quests: 42 | Completed : 0 | Remaining: 42 |</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="str">
+        <f>"Dueling Peaks Region ("&amp;COUNTIF(B5:B11,"Yes")&amp;"/11)"</f>
+        <v>Dueling Peaks Region (0/11)</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="F4" s="6" t="str">
+        <f>"Hateno Region ("&amp;COUNTIF(F5:F9,"Yes")&amp;"/10)"</f>
+        <v>Hateno Region (0/10)</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="J4" s="6" t="str">
+        <f>"Central Region ("&amp;COUNTIF(J5:J9,"Yes")&amp;"/5)"</f>
+        <v>Central Region (0/5)</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="e">
+        <f>IF(VLOOKUP(C5,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="e">
+        <f>IF(VLOOKUP(G5,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <f>IF(VLOOKUP(K5,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="e">
+        <f>IF(VLOOKUP(C6,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F6" s="2" t="e">
+        <f>IF(VLOOKUP(G6,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <f>IF(VLOOKUP(K6,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="e">
+        <f>IF(VLOOKUP(G7,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <f>IF(VLOOKUP(K7,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="str">
+        <f>"Lanayru Region ("&amp;COUNTIF(B9:B26,"Yes")&amp;"/9)"</f>
+        <v>Lanayru Region (0/9)</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="F8" s="2" t="e">
+        <f>IF(VLOOKUP(G8,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <f>IF(VLOOKUP(K8,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="e">
+        <f>IF(VLOOKUP(C9,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="e">
+        <f>IF(VLOOKUP(C10,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="6" t="str">
+        <f>"Wasteland Region ("&amp;COUNTIF(F11:F28,"Yes")&amp;"/12)"</f>
+        <v>Wasteland Region (0/12)</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="J10" s="6" t="str">
+        <f>"Eldin Region ("&amp;COUNTIF(J11:J14,"Yes")&amp;"/4)"</f>
+        <v>Eldin Region (0/4)</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="e">
+        <f>IF(VLOOKUP(G11,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J11" s="2" t="e">
+        <f>IF(VLOOKUP(K11,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="str">
+        <f>"Faron Region ("&amp;COUNTIF(B13:B33,"Yes")&amp;"/5)"</f>
+        <v>Faron Region (0/5)</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="F12" s="2" t="e">
+        <f>IF(VLOOKUP(G12,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J12" s="2" t="e">
+        <f>IF(VLOOKUP(K12,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="e">
+        <f>IF(VLOOKUP(C13,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" s="2" t="e">
+        <f>IF(VLOOKUP(G13,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J13" s="2" t="e">
+        <f>IF(VLOOKUP(K13,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="e">
+        <f>IF(VLOOKUP(C14,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F14" s="2" t="e">
+        <f>IF(VLOOKUP(G14,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="e">
+        <f>IF(VLOOKUP(C15,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F15" s="2" t="e">
+        <f>IF(VLOOKUP(G15,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="6" t="str">
+        <f>"Tabantha Region ("&amp;COUNTIF(J16:J22,"Yes")&amp;"/6)"</f>
+        <v>Tabantha Region (0/6)</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="e">
+        <f>IF(VLOOKUP(C16,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F16" s="2" t="e">
+        <f>IF(VLOOKUP(G16,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J16" s="2" t="e">
+        <f>IF(VLOOKUP(K16,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="e">
+        <f>IF(VLOOKUP(G17,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J17" s="2" t="e">
+        <f>IF(VLOOKUP(K17,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="str">
+        <f>"Woodland Region ("&amp;COUNTIF(F31:F37,"Yes")&amp;"/7)"</f>
+        <v>Woodland Region (0/7)</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="F18" s="2" t="e">
+        <f>IF(VLOOKUP(G18,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="e">
+        <f>IF(VLOOKUP(C19,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F19" s="2" t="e">
+        <f>IF(VLOOKUP(G19,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="6" t="str">
+        <f>"Lake Region ("&amp;COUNTIF(J20:J21,"Yes")&amp;"/2)"</f>
+        <v>Lake Region (0/2)</v>
+      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="e">
+        <f>IF(VLOOKUP(C20,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F20" s="2" t="e">
+        <f>IF(VLOOKUP(G20,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J20" s="2" t="e">
+        <f>IF(VLOOKUP(K20,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="e">
+        <f>IF(VLOOKUP(C21,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J21" s="2" t="e">
+        <f>IF(VLOOKUP(K21,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F22" s="6" t="str">
+        <f>"Akkala Region ("&amp;COUNTIF(F23:F26,"Yes")&amp;"/4)"</f>
+        <v>Akkala Region (0/4)</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="str">
+        <f>"Hebra Region ("&amp;COUNTIF(B24:B25,"Yes")&amp;"/2)"</f>
+        <v>Hebra Region (0/2)</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="F23" s="2" t="e">
+        <f>IF(VLOOKUP(G23,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="e">
+        <f>IF(VLOOKUP(C24,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="2" t="e">
+        <f>IF(VLOOKUP(G24,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="e">
+        <f>IF(VLOOKUP(C25,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F25" s="2" t="e">
+        <f>IF(VLOOKUP(G25,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="e">
+        <f>IF(VLOOKUP(G26,Savegame_Data!$A:$E,5,FALSE)=1,"Yes","No")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="J10:L10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B2:G2 I2:L2 B49:L1048576 E38:L48 B27:I27 I24:I26 E17:E26 B3:L9 B10:E16 F10:H20 J10:L13 I20:L23 I10:I19 J15:L17 E28:I29 E30:E37 I30:I33 B18:D21 J19:L21 J28:L28 F22:H25 I34:L34 I35:I37 B23:D25">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:D26">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:D33">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34:H37">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:D48">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26:H26">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAE7648-3E67-41C5-8AFB-B722B117B233}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>